<commit_message>
change way detect apollo as object'
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/week10/Huy Nguyen Week 10 Timesheet .xlsx
+++ b/Documentation/TimeSheets/week10/Huy Nguyen Week 10 Timesheet .xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Hours Worked</t>
   </si>
@@ -122,6 +122,15 @@
   </si>
   <si>
     <t>6:00PM</t>
+  </si>
+  <si>
+    <t>Coding Auto Survey - Avoid NGZ</t>
+  </si>
+  <si>
+    <t>9:00AM</t>
+  </si>
+  <si>
+    <t>1:00PM</t>
   </si>
 </sst>
 </file>
@@ -294,7 +303,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -341,6 +350,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="8" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -737,7 +752,7 @@
   <dimension ref="B1:H19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -799,15 +814,15 @@
       </c>
       <c r="C5" s="8">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>10.5</v>
+        <v>14.5</v>
       </c>
       <c r="D5" s="8">
         <f>IFERROR(IF(C5&lt;=WorkweekHours,C5,WorkweekHours),"")</f>
-        <v>10.5</v>
+        <v>12</v>
       </c>
       <c r="E5" s="8">
         <f>IFERROR(C5-D5, "")</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -927,11 +942,21 @@
       </c>
     </row>
     <row r="13" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="10"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
+      <c r="B13" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="13">
+        <v>43053</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="12">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>

</xml_diff>